<commit_message>
Updated interval in gss
</commit_message>
<xml_diff>
--- a/Report_Second_Pearson.xlsx
+++ b/Report_Second_Pearson.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,29 +485,29 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>150</v>
+        <v>-0.6914893617021276</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6262385173353626</v>
+        <v>6.332875812655695</v>
       </c>
       <c r="F2" t="n">
-        <v>-11.89853182937191</v>
+        <v>2.162561938137853</v>
       </c>
       <c r="G2" t="n">
-        <v>-2.504954069341535</v>
+        <v>1.224384658965657</v>
       </c>
       <c r="H2" t="n">
-        <v>-118.0473421765202</v>
+        <v>-2.339012326833017</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[19.  4.]</t>
+          <t>[-0.34148182 -0.19333786]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -522,35 +522,35 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.898531829371914</v>
+        <v>2.162561938137853</v>
       </c>
       <c r="C3" t="n">
-        <v>7.495045930658465</v>
+        <v>1.224384658965657</v>
       </c>
       <c r="D3" t="n">
-        <v>31.9526578234798</v>
+        <v>-3.030501688535145</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3658447905295747</v>
+        <v>0.1905886164704917</v>
       </c>
       <c r="F3" t="n">
-        <v>2.014009388570326</v>
+        <v>-0.2672761957678043</v>
       </c>
       <c r="G3" t="n">
-        <v>-2.808093217310844</v>
+        <v>0.106238753696128</v>
       </c>
       <c r="H3" t="n">
-        <v>-17.59545312636053</v>
+        <v>-0.1689365886072731</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[-2.29210959 10.88862369]</t>
+          <t>[ 0.70846967 -1.25132707]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[[ 0.62624585 -0.37375415]
- [-0.37375415  0.62624585]]</t>
+          <t>[[-0.27824109 -1.27824109]
+ [-1.27824109 -0.27824109]]</t>
         </is>
       </c>
     </row>
@@ -559,35 +559,35 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1154775591984127</v>
+        <v>1.895285742370049</v>
       </c>
       <c r="C4" t="n">
-        <v>4.686952713347621</v>
+        <v>1.330623412661785</v>
       </c>
       <c r="D4" t="n">
-        <v>14.35720469711928</v>
+        <v>-3.199438277142418</v>
       </c>
       <c r="E4" t="n">
-        <v>3.305348067594794e-05</v>
+        <v>0.968471816849644</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0001148595726403606</v>
+        <v>0.4856429525147876</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001573522857745147</v>
+        <v>1.221772422944872</v>
       </c>
       <c r="H4" t="n">
-        <v>0.001034663126347368</v>
+        <v>-0.9008737583491855</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[4.54400241 3.25842787]</t>
+          <t>[-0.50145285 -1.2615467 ]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[[-0.02775207 -1.02775207]
- [-1.02775207 -0.02775207]]</t>
+          <t>[[1 0]
+ [0 1]]</t>
         </is>
       </c>
     </row>
@@ -596,35 +596,35 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1155924187710531</v>
+        <v>2.380928694884836</v>
       </c>
       <c r="C5" t="n">
-        <v>4.687110065633395</v>
+        <v>2.552395835606657</v>
       </c>
       <c r="D5" t="n">
-        <v>14.35823936024562</v>
+        <v>-4.100312035491603</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3720560305598584</v>
+        <v>0.09450915975475314</v>
       </c>
       <c r="F5" t="n">
-        <v>-4.135910026981164</v>
+        <v>0.01234619452251717</v>
       </c>
       <c r="G5" t="n">
-        <v>-3.657651696561127</v>
+        <v>0.229808688093986</v>
       </c>
       <c r="H5" t="n">
-        <v>-15.35636023593253</v>
+        <v>-0.07252651155991163</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[4.54407477 3.25862771]</t>
+          <t>[ 1.64649999 -0.65446739]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[[1.84230926 0.84230926]
- [0.84230926 1.84230926]]</t>
+          <t>[[-0.79140775 -1.79140775]
+ [-1.79140775 -0.79140775]]</t>
         </is>
       </c>
     </row>
@@ -633,35 +633,35 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-4.020317608210111</v>
+        <v>2.393274889407353</v>
       </c>
       <c r="C6" t="n">
-        <v>1.029458369072268</v>
+        <v>2.782204523700643</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.998120875686908</v>
+        <v>-4.172838547051515</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3323091444885113</v>
+        <v>0.2551557195878111</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02581676103435226</v>
+        <v>-0.3914645252374407</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.02380627624600806</v>
+        <v>0.02103609680670449</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.001848019200217266</v>
+        <v>-0.3359251546719575</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[-0.07009359  0.07923435]</t>
+          <t>[ 1.53421811 -0.08244415]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[[ 0.16906237 -0.83093763]
- [-0.83093763  0.16906237]]</t>
+          <t>[[1 0]
+ [0 1]]</t>
         </is>
       </c>
     </row>
@@ -670,35 +670,35 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-3.994500847175759</v>
+        <v>2.001810364169913</v>
       </c>
       <c r="C7" t="n">
-        <v>1.00565209282626</v>
+        <v>2.803240620507347</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.9999688948871253</v>
+        <v>-4.508763701723472</v>
       </c>
       <c r="E7" t="n">
-        <v>3.305348067594794e-05</v>
+        <v>4.348389486982408e-06</v>
       </c>
       <c r="F7" t="n">
-        <v>3.74817902493163e-07</v>
+        <v>2.18805851526227e-06</v>
       </c>
       <c r="G7" t="n">
-        <v>3.596523041604627e-07</v>
+        <v>1.513455606616532e-06</v>
       </c>
       <c r="H7" t="n">
-        <v>4.091781136139616e-09</v>
+        <v>2.673845518330609e-07</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>[0.00534621 0.00580503]</t>
+          <t>[0.00880003 0.16393859]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[[-0.49633091 -1.49633091]
- [-1.49633091 -0.49633091]]</t>
+          <t>[[-1.96394799 -2.96394799]
+ [-2.96394799 -1.96394799]]</t>
         </is>
       </c>
     </row>
@@ -707,35 +707,183 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.994500472357856</v>
+        <v>2.001812552228428</v>
       </c>
       <c r="C8" t="n">
-        <v>1.005652452478564</v>
+        <v>2.803242133962954</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.9999688907953441</v>
+        <v>-4.50876343433892</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2510690638920298</v>
+        <v>0.2855843683986543</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.005518881038242718</v>
+        <v>-0.002516185200630794</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.005634065124823007</v>
+        <v>-0.04681987327169557</v>
       </c>
       <c r="H8" t="n">
-        <v>-3.110813614881636e-05</v>
+        <v>-0.003792593412013545</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[0.0053466  0.00580538]</t>
+          <t>[0.00881065 0.1639441 ]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[[2.49165642 1.49165642]
- [1.49165642 2.49165642]]</t>
+          <t>[[1 0]
+ [0 1]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.999296367027797</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.756422260691259</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-4.512556027750934</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4.348389486982408e-06</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-2.08827362069286e-08</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-3.696812633791069e-08</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.630518356587345e-11</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>[-0.00350993  0.00018923]</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>[[-1.50318452 -2.50318452]
+ [-2.50318452 -1.50318452]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.999296346145061</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.756422223723132</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-4.512556027684629</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.2006694148189</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0007043571775595669</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-3.794731176931521e-05</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-1.239721843404595e-06</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>[-0.00351004  0.0001891 ]</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>[[1 0]
+ [0 1]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2.000000703322621</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.756384276411363</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-4.512557267406472</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.348389486982408e-06</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.138163341352083e-09</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8.792420125303124e-10</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5.950795411990839e-14</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>[3.50845938e-06 6.30527433e-05]</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>[[-2.9850866 -3.9850866]
+ [-3.9850866 -2.9850866]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.000000704460784</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.756384277290605</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-4.512557267406413</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.29914064386528</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-1.05122121807355e-06</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-1.88625164203593e-05</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-5.963265437003429e-10</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>[3.51413704e-06 6.30556790e-05]</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>[[1 0]
+ [0 1]]</t>
         </is>
       </c>
     </row>

</xml_diff>